<commit_message>
200704 02:47 ignore nulls
</commit_message>
<xml_diff>
--- a/tiankx/data/demo.xlsx
+++ b/tiankx/data/demo.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\TechSummary\tiankx\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E051E99-3E69-4ED6-8560-1AE3CEE43B3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657739FA-610C-4E00-9E6D-39232EC55971}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quotation_info" sheetId="1" r:id="rId1"/>
     <sheet name="quotation_smooth" sheetId="3" r:id="rId2"/>
+    <sheet name="quotation_ext" sheetId="4" r:id="rId3"/>
+    <sheet name="quotation_ext_smooth" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="465">
   <si>
     <t>the_date</t>
   </si>
@@ -388,6 +390,1053 @@
   <si>
     <t>2020-02-01</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> value3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> value4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> value5</t>
+  </si>
+  <si>
+    <t>2020-01-01</t>
+  </si>
+  <si>
+    <t>527.3998275</t>
+  </si>
+  <si>
+    <t>751.8710904</t>
+  </si>
+  <si>
+    <t>106.948547</t>
+  </si>
+  <si>
+    <t>23396.02276</t>
+  </si>
+  <si>
+    <t>1007.645957</t>
+  </si>
+  <si>
+    <t>2020-01-02</t>
+  </si>
+  <si>
+    <t>505.5326139</t>
+  </si>
+  <si>
+    <t>504.738142</t>
+  </si>
+  <si>
+    <t>194.5720481</t>
+  </si>
+  <si>
+    <t>11140.77039</t>
+  </si>
+  <si>
+    <t>1002.489356</t>
+  </si>
+  <si>
+    <t>2020-01-03</t>
+  </si>
+  <si>
+    <t>524.7400722</t>
+  </si>
+  <si>
+    <t>717.6718156</t>
+  </si>
+  <si>
+    <t>167.4062059</t>
+  </si>
+  <si>
+    <t>943.3793967</t>
+  </si>
+  <si>
+    <t>1005.140107</t>
+  </si>
+  <si>
+    <t>2020-01-04</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>105.3210817</t>
+  </si>
+  <si>
+    <t>3598.221718</t>
+  </si>
+  <si>
+    <t>2020-01-05</t>
+  </si>
+  <si>
+    <t>691.9463228</t>
+  </si>
+  <si>
+    <t>164.0813652</t>
+  </si>
+  <si>
+    <t>28750.87484</t>
+  </si>
+  <si>
+    <t>999.5027359</t>
+  </si>
+  <si>
+    <t>908.5412257</t>
+  </si>
+  <si>
+    <t>182.6815502</t>
+  </si>
+  <si>
+    <t>1008.846711</t>
+  </si>
+  <si>
+    <t>491.1317648</t>
+  </si>
+  <si>
+    <t>115.2530362</t>
+  </si>
+  <si>
+    <t>10267.09424</t>
+  </si>
+  <si>
+    <t>1002.268034</t>
+  </si>
+  <si>
+    <t>500.2062626</t>
+  </si>
+  <si>
+    <t>24235.95141</t>
+  </si>
+  <si>
+    <t>1006.137574</t>
+  </si>
+  <si>
+    <t>470.5343541</t>
+  </si>
+  <si>
+    <t>6614.27531</t>
+  </si>
+  <si>
+    <t>1004.342238</t>
+  </si>
+  <si>
+    <t>981.2035901</t>
+  </si>
+  <si>
+    <t>18832.26594</t>
+  </si>
+  <si>
+    <t>2020-01-11</t>
+  </si>
+  <si>
+    <t>18134.16471</t>
+  </si>
+  <si>
+    <t>126.7927798</t>
+  </si>
+  <si>
+    <t>20099.10184</t>
+  </si>
+  <si>
+    <t>124.5343908</t>
+  </si>
+  <si>
+    <t>23833.61227</t>
+  </si>
+  <si>
+    <t>178.5977257</t>
+  </si>
+  <si>
+    <t>1003.118354</t>
+  </si>
+  <si>
+    <t>175.2717636</t>
+  </si>
+  <si>
+    <t>999.145431</t>
+  </si>
+  <si>
+    <t>151.0381951</t>
+  </si>
+  <si>
+    <t>1000.111845</t>
+  </si>
+  <si>
+    <t>164.5369872</t>
+  </si>
+  <si>
+    <t>1003.852623</t>
+  </si>
+  <si>
+    <t>2020-01-18</t>
+  </si>
+  <si>
+    <t>383.1379687</t>
+  </si>
+  <si>
+    <t>100.0736913</t>
+  </si>
+  <si>
+    <t>1003.518364</t>
+  </si>
+  <si>
+    <t>795.7181297</t>
+  </si>
+  <si>
+    <t>188.2834512</t>
+  </si>
+  <si>
+    <t>1000.960012</t>
+  </si>
+  <si>
+    <t>756.5973352</t>
+  </si>
+  <si>
+    <t>108.3384304</t>
+  </si>
+  <si>
+    <t>1002.386925</t>
+  </si>
+  <si>
+    <t>301.4501776</t>
+  </si>
+  <si>
+    <t>114.7042222</t>
+  </si>
+  <si>
+    <t>1007.048534</t>
+  </si>
+  <si>
+    <t>502.9957055</t>
+  </si>
+  <si>
+    <t>298.1549422</t>
+  </si>
+  <si>
+    <t>181.0232838</t>
+  </si>
+  <si>
+    <t>999.8189345</t>
+  </si>
+  <si>
+    <t>518.6823174</t>
+  </si>
+  <si>
+    <t>304.9583119</t>
+  </si>
+  <si>
+    <t>183.7222096</t>
+  </si>
+  <si>
+    <t>1006.978465</t>
+  </si>
+  <si>
+    <t>524.7262836</t>
+  </si>
+  <si>
+    <t>147.9061556</t>
+  </si>
+  <si>
+    <t>882.4792794</t>
+  </si>
+  <si>
+    <t>1005.993532</t>
+  </si>
+  <si>
+    <t>2020-01-25</t>
+  </si>
+  <si>
+    <t>503.1531049</t>
+  </si>
+  <si>
+    <t>101.4407648</t>
+  </si>
+  <si>
+    <t>9224.259585</t>
+  </si>
+  <si>
+    <t>1000.382231</t>
+  </si>
+  <si>
+    <t>508.0334657</t>
+  </si>
+  <si>
+    <t>103.4829745</t>
+  </si>
+  <si>
+    <t>5502.879129</t>
+  </si>
+  <si>
+    <t>1000.26354</t>
+  </si>
+  <si>
+    <t>529.0343859</t>
+  </si>
+  <si>
+    <t>158.9883112</t>
+  </si>
+  <si>
+    <t>20785.35544</t>
+  </si>
+  <si>
+    <t>1003.102037</t>
+  </si>
+  <si>
+    <t>531.2297385</t>
+  </si>
+  <si>
+    <t>141.1106538</t>
+  </si>
+  <si>
+    <t>9431.683865</t>
+  </si>
+  <si>
+    <t>1007.351911</t>
+  </si>
+  <si>
+    <t>176.6257337</t>
+  </si>
+  <si>
+    <t>11386.48962</t>
+  </si>
+  <si>
+    <t>128.8957849</t>
+  </si>
+  <si>
+    <t>19652.8611</t>
+  </si>
+  <si>
+    <t>1005.396158</t>
+  </si>
+  <si>
+    <t>794.4905671</t>
+  </si>
+  <si>
+    <t>190.7297652</t>
+  </si>
+  <si>
+    <t>24935.34942</t>
+  </si>
+  <si>
+    <t>999.9732889</t>
+  </si>
+  <si>
+    <t>2020-02-01</t>
+  </si>
+  <si>
+    <t>346.4294547</t>
+  </si>
+  <si>
+    <t>135.7651354</t>
+  </si>
+  <si>
+    <t>4083.093607</t>
+  </si>
+  <si>
+    <t>1000.425783</t>
+  </si>
+  <si>
+    <t>103.3708197</t>
+  </si>
+  <si>
+    <t>112.728912</t>
+  </si>
+  <si>
+    <t>24140.88986</t>
+  </si>
+  <si>
+    <t>1005.04353</t>
+  </si>
+  <si>
+    <t>62.76440654</t>
+  </si>
+  <si>
+    <t>161.41475</t>
+  </si>
+  <si>
+    <t>2809.450411</t>
+  </si>
+  <si>
+    <t>1008.441789</t>
+  </si>
+  <si>
+    <t>504.0929537</t>
+  </si>
+  <si>
+    <t>418.3444823</t>
+  </si>
+  <si>
+    <t>149.3373395</t>
+  </si>
+  <si>
+    <t>27156.69815</t>
+  </si>
+  <si>
+    <t>1007.246705</t>
+  </si>
+  <si>
+    <t>512.931405</t>
+  </si>
+  <si>
+    <t>614.6123742</t>
+  </si>
+  <si>
+    <t>110.6416895</t>
+  </si>
+  <si>
+    <t>12683.98289</t>
+  </si>
+  <si>
+    <t>1001.214602</t>
+  </si>
+  <si>
+    <t>516.9544361</t>
+  </si>
+  <si>
+    <t>396.9120707</t>
+  </si>
+  <si>
+    <t>193.9040587</t>
+  </si>
+  <si>
+    <t>761.6074194</t>
+  </si>
+  <si>
+    <t>1007.926196</t>
+  </si>
+  <si>
+    <t>501.6928866</t>
+  </si>
+  <si>
+    <t>216.2225743</t>
+  </si>
+  <si>
+    <t>171.2128189</t>
+  </si>
+  <si>
+    <t>23875.08059</t>
+  </si>
+  <si>
+    <t>1005.046161</t>
+  </si>
+  <si>
+    <t>2020-02-08</t>
+  </si>
+  <si>
+    <t>511.6414903</t>
+  </si>
+  <si>
+    <t>58.45023774</t>
+  </si>
+  <si>
+    <t>168.9434576</t>
+  </si>
+  <si>
+    <t>6955.047916</t>
+  </si>
+  <si>
+    <t>1000.152672</t>
+  </si>
+  <si>
+    <t>2020-02-09</t>
+  </si>
+  <si>
+    <t>985.6192616</t>
+  </si>
+  <si>
+    <t>111.2029843</t>
+  </si>
+  <si>
+    <t>22630.6189</t>
+  </si>
+  <si>
+    <t>2020-02-10</t>
+  </si>
+  <si>
+    <t>521.8639121</t>
+  </si>
+  <si>
+    <t>169.6267219</t>
+  </si>
+  <si>
+    <t>124.2119556</t>
+  </si>
+  <si>
+    <t>15370.61844</t>
+  </si>
+  <si>
+    <t>1004.006206</t>
+  </si>
+  <si>
+    <t>2020-02-11</t>
+  </si>
+  <si>
+    <t>504.7573915</t>
+  </si>
+  <si>
+    <t>744.7551325</t>
+  </si>
+  <si>
+    <t>5363.818993</t>
+  </si>
+  <si>
+    <t>999.6001808</t>
+  </si>
+  <si>
+    <t>2020-02-12</t>
+  </si>
+  <si>
+    <t>521.0418803</t>
+  </si>
+  <si>
+    <t>757.9314781</t>
+  </si>
+  <si>
+    <t>190.9993381</t>
+  </si>
+  <si>
+    <t>1279.329414</t>
+  </si>
+  <si>
+    <t>1006.562612</t>
+  </si>
+  <si>
+    <t>2020-02-13</t>
+  </si>
+  <si>
+    <t>501.8623486</t>
+  </si>
+  <si>
+    <t>867.5383864</t>
+  </si>
+  <si>
+    <t>151.6302696</t>
+  </si>
+  <si>
+    <t>20773.90466</t>
+  </si>
+  <si>
+    <t>1002.990717</t>
+  </si>
+  <si>
+    <t>2020-02-14</t>
+  </si>
+  <si>
+    <t>502.502914</t>
+  </si>
+  <si>
+    <t>291.8007728</t>
+  </si>
+  <si>
+    <t>175.2016195</t>
+  </si>
+  <si>
+    <t>5668.741689</t>
+  </si>
+  <si>
+    <t>1006.769581</t>
+  </si>
+  <si>
+    <t>2020-02-15</t>
+  </si>
+  <si>
+    <t>505.6234565</t>
+  </si>
+  <si>
+    <t>778.3326911</t>
+  </si>
+  <si>
+    <t>113.8208615</t>
+  </si>
+  <si>
+    <t>11865.21884</t>
+  </si>
+  <si>
+    <t>1006.827953</t>
+  </si>
+  <si>
+    <t>2020-02-16</t>
+  </si>
+  <si>
+    <t>527.8329375</t>
+  </si>
+  <si>
+    <t>469.4248217</t>
+  </si>
+  <si>
+    <t>117.2823204</t>
+  </si>
+  <si>
+    <t>25617.48373</t>
+  </si>
+  <si>
+    <t>999.86879</t>
+  </si>
+  <si>
+    <t>2020-02-17</t>
+  </si>
+  <si>
+    <t>518.1600494</t>
+  </si>
+  <si>
+    <t>255.841999</t>
+  </si>
+  <si>
+    <t>122.4226271</t>
+  </si>
+  <si>
+    <t>23441.52846</t>
+  </si>
+  <si>
+    <t>1001.856486</t>
+  </si>
+  <si>
+    <t>2020-02-18</t>
+  </si>
+  <si>
+    <t>530.1081296</t>
+  </si>
+  <si>
+    <t>217.6452884</t>
+  </si>
+  <si>
+    <t>141.9519288</t>
+  </si>
+  <si>
+    <t>1006.300253</t>
+  </si>
+  <si>
+    <t>2020-02-19</t>
+  </si>
+  <si>
+    <t>503.7999647</t>
+  </si>
+  <si>
+    <t>91.65992509</t>
+  </si>
+  <si>
+    <t>154.4191281</t>
+  </si>
+  <si>
+    <t>631.5618216</t>
+  </si>
+  <si>
+    <t>2020-02-20</t>
+  </si>
+  <si>
+    <t>504.0564852</t>
+  </si>
+  <si>
+    <t>258.5167842</t>
+  </si>
+  <si>
+    <t>134.0066431</t>
+  </si>
+  <si>
+    <t>5600.709921</t>
+  </si>
+  <si>
+    <t>1003.757315</t>
+  </si>
+  <si>
+    <t>2020-02-21</t>
+  </si>
+  <si>
+    <t>509.7950626</t>
+  </si>
+  <si>
+    <t>946.8517138</t>
+  </si>
+  <si>
+    <t>196.7482582</t>
+  </si>
+  <si>
+    <t>5094.747329</t>
+  </si>
+  <si>
+    <t>1006.836871</t>
+  </si>
+  <si>
+    <t>2020-02-22</t>
+  </si>
+  <si>
+    <t>514.2349563</t>
+  </si>
+  <si>
+    <t>311.61993</t>
+  </si>
+  <si>
+    <t>121.5586274</t>
+  </si>
+  <si>
+    <t>28341.07571</t>
+  </si>
+  <si>
+    <t>1001.159775</t>
+  </si>
+  <si>
+    <t>2020-02-23</t>
+  </si>
+  <si>
+    <t>502.6477952</t>
+  </si>
+  <si>
+    <t>995.5941488</t>
+  </si>
+  <si>
+    <t>189.0072106</t>
+  </si>
+  <si>
+    <t>25167.80482</t>
+  </si>
+  <si>
+    <t>1004.511638</t>
+  </si>
+  <si>
+    <t>2020-02-24</t>
+  </si>
+  <si>
+    <t>529.180962</t>
+  </si>
+  <si>
+    <t>507.9345606</t>
+  </si>
+  <si>
+    <t>116.4197564</t>
+  </si>
+  <si>
+    <t>18483.28678</t>
+  </si>
+  <si>
+    <t>1002.730031</t>
+  </si>
+  <si>
+    <t>2020-02-25</t>
+  </si>
+  <si>
+    <t>74.52877538</t>
+  </si>
+  <si>
+    <t>154.3444529</t>
+  </si>
+  <si>
+    <t>759.8672738</t>
+  </si>
+  <si>
+    <t>1005.547884</t>
+  </si>
+  <si>
+    <t>2020-02-26</t>
+  </si>
+  <si>
+    <t>114.4126366</t>
+  </si>
+  <si>
+    <t>172.8595598</t>
+  </si>
+  <si>
+    <t>28998.8837</t>
+  </si>
+  <si>
+    <t>1008.315435</t>
+  </si>
+  <si>
+    <t>2020-02-27</t>
+  </si>
+  <si>
+    <t>501.9411086</t>
+  </si>
+  <si>
+    <t>175.6085119</t>
+  </si>
+  <si>
+    <t>24607.05999</t>
+  </si>
+  <si>
+    <t>1002.448217</t>
+  </si>
+  <si>
+    <t>2020-02-28</t>
+  </si>
+  <si>
+    <t>159.317453</t>
+  </si>
+  <si>
+    <t>120.4788554</t>
+  </si>
+  <si>
+    <t>8007.490084</t>
+  </si>
+  <si>
+    <t>1006.791579</t>
+  </si>
+  <si>
+    <t>2020-02-29</t>
+  </si>
+  <si>
+    <t>403.889757</t>
+  </si>
+  <si>
+    <t>194.7773512</t>
+  </si>
+  <si>
+    <t>18142.92421</t>
+  </si>
+  <si>
+    <t>1001.243004</t>
+  </si>
+  <si>
+    <t>2020-03-01</t>
+  </si>
+  <si>
+    <t>565.3862225</t>
+  </si>
+  <si>
+    <t>150.8756074</t>
+  </si>
+  <si>
+    <t>15393.62699</t>
+  </si>
+  <si>
+    <t>1008.659847</t>
+  </si>
+  <si>
+    <t>2020-03-02</t>
+  </si>
+  <si>
+    <t>181.423187</t>
+  </si>
+  <si>
+    <t>164.2022233</t>
+  </si>
+  <si>
+    <t>2775.78337</t>
+  </si>
+  <si>
+    <t>1005.09946</t>
+  </si>
+  <si>
+    <t>2020-03-03</t>
+  </si>
+  <si>
+    <t>998.4135137</t>
+  </si>
+  <si>
+    <t>131.8928102</t>
+  </si>
+  <si>
+    <t>22053.3365</t>
+  </si>
+  <si>
+    <t>999.6826394</t>
+  </si>
+  <si>
+    <t>2020-03-04</t>
+  </si>
+  <si>
+    <t>254.5957446</t>
+  </si>
+  <si>
+    <t>126.6521443</t>
+  </si>
+  <si>
+    <t>17054.00309</t>
+  </si>
+  <si>
+    <t>1005.258035</t>
+  </si>
+  <si>
+    <t>2020-03-05</t>
+  </si>
+  <si>
+    <t>137.6091437</t>
+  </si>
+  <si>
+    <t>103.1375005</t>
+  </si>
+  <si>
+    <t>10929.21458</t>
+  </si>
+  <si>
+    <t>1003.996882</t>
+  </si>
+  <si>
+    <t>2020-03-06</t>
+  </si>
+  <si>
+    <t>869.9321248</t>
+  </si>
+  <si>
+    <t>146.047399</t>
+  </si>
+  <si>
+    <t>16210.53447</t>
+  </si>
+  <si>
+    <t>1000.653353</t>
+  </si>
+  <si>
+    <t>2020-03-07</t>
+  </si>
+  <si>
+    <t>338.0127601</t>
+  </si>
+  <si>
+    <t>176.8739934</t>
+  </si>
+  <si>
+    <t>19029.37002</t>
+  </si>
+  <si>
+    <t>1007.982856</t>
+  </si>
+  <si>
+    <t>2020-03-08</t>
+  </si>
+  <si>
+    <t>86.60383319</t>
+  </si>
+  <si>
+    <t>138.9962828</t>
+  </si>
+  <si>
+    <t>25689.79891</t>
+  </si>
+  <si>
+    <t>1008.537934</t>
+  </si>
+  <si>
+    <t>2020-03-09</t>
+  </si>
+  <si>
+    <t>317.2204428</t>
+  </si>
+  <si>
+    <t>142.4398642</t>
+  </si>
+  <si>
+    <t>23013.87218</t>
+  </si>
+  <si>
+    <t>1008.814238</t>
+  </si>
+  <si>
+    <t>2020-03-10</t>
+  </si>
+  <si>
+    <t>509.7650785</t>
+  </si>
+  <si>
+    <t>455.2288575</t>
+  </si>
+  <si>
+    <t>195.3181398</t>
+  </si>
+  <si>
+    <t>26457.95592</t>
+  </si>
+  <si>
+    <t>1005.094478</t>
+  </si>
+  <si>
+    <t>2020-03-11</t>
+  </si>
+  <si>
+    <t>503.5552106</t>
+  </si>
+  <si>
+    <t>508.6802691</t>
+  </si>
+  <si>
+    <t>187.4318985</t>
+  </si>
+  <si>
+    <t>20835.16288</t>
+  </si>
+  <si>
+    <t>1005.223595</t>
+  </si>
+  <si>
+    <t>524.7400723</t>
+  </si>
+  <si>
+    <t>524.7400724</t>
+  </si>
+  <si>
+    <t>524.7400725</t>
+  </si>
+  <si>
+    <t>524.7400726</t>
+  </si>
+  <si>
+    <t>524.7400727</t>
+  </si>
+  <si>
+    <t>524.7400728</t>
+  </si>
+  <si>
+    <t>524.7400729</t>
+  </si>
+  <si>
+    <t>524.7400730</t>
+  </si>
+  <si>
+    <t>524.7400731</t>
+  </si>
+  <si>
+    <t>524.7400732</t>
+  </si>
+  <si>
+    <t>23833.61228</t>
+  </si>
+  <si>
+    <t>524.7400733</t>
+  </si>
+  <si>
+    <t>23833.61229</t>
+  </si>
+  <si>
+    <t>524.7400734</t>
+  </si>
+  <si>
+    <t>23833.61230</t>
+  </si>
+  <si>
+    <t>524.7400735</t>
+  </si>
+  <si>
+    <t>23833.61231</t>
+  </si>
+  <si>
+    <t>524.7400736</t>
+  </si>
+  <si>
+    <t>23833.61232</t>
+  </si>
+  <si>
+    <t>524.7400737</t>
+  </si>
+  <si>
+    <t>23833.61233</t>
+  </si>
+  <si>
+    <t>524.7400738</t>
+  </si>
+  <si>
+    <t>23833.61234</t>
+  </si>
+  <si>
+    <t>524.7400739</t>
+  </si>
+  <si>
+    <t>23833.61235</t>
+  </si>
+  <si>
+    <t>23833.61236</t>
+  </si>
+  <si>
+    <t>23833.61237</t>
   </si>
 </sst>
 </file>
@@ -419,7 +1468,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -444,6 +1493,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -457,13 +1512,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1133,8 +2189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0992A8-0716-4F2E-AE52-00D295829E1D}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1872,4 +2928,3359 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E4A6D7B-B959-4D94-83A6-DD3DE7A85DF4}">
+  <dimension ref="A1:G72"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B78251BD-66C0-4F23-9027-988DFB054FCE}">
+  <dimension ref="A1:G72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>